<commit_message>
win32com high quality PDF
</commit_message>
<xml_diff>
--- a/app/core/testing.xlsx
+++ b/app/core/testing.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master of IT\Semester4\software project\DC-Boxjelly\app\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8563AE57-1CB4-403E-956F-CE9D29F360B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F34D574-B9E3-4FE5-A3F4-50DFD6A6D3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="180" windowWidth="17280" windowHeight="11580" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MEXReport" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -366,6 +369,195 @@
     <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
+    <t>(-250) on the guard electrode Positive (Central Electrode Negative)</t>
+  </si>
+  <si>
+    <t>NXA50</t>
+  </si>
+  <si>
+    <t>NXA70</t>
+  </si>
+  <si>
+    <t>NXB100</t>
+  </si>
+  <si>
+    <t>NXC120</t>
+  </si>
+  <si>
+    <t>NXD140</t>
+  </si>
+  <si>
+    <t>NXE150</t>
+  </si>
+  <si>
+    <t>NXF200</t>
+  </si>
+  <si>
+    <t>NXG250</t>
+  </si>
+  <si>
+    <t>NXH280</t>
+  </si>
+  <si>
+    <t>NXH300</t>
+  </si>
+  <si>
+    <t>NXH300*</t>
+  </si>
+  <si>
+    <t>NXJ40</t>
+  </si>
+  <si>
+    <t>NXK40</t>
+  </si>
+  <si>
+    <t>NXA40</t>
+  </si>
+  <si>
+    <t>NXJ50</t>
+  </si>
+  <si>
+    <t>NXK50</t>
+  </si>
+  <si>
+    <t>NXB50</t>
+  </si>
+  <si>
+    <t>NXJ60</t>
+  </si>
+  <si>
+    <t>NXK60</t>
+  </si>
+  <si>
+    <t>NXA60</t>
+  </si>
+  <si>
+    <t>NXJ70</t>
+  </si>
+  <si>
+    <t>NXK70</t>
+  </si>
+  <si>
+    <t>NXB70</t>
+  </si>
+  <si>
+    <t>NXC70</t>
+  </si>
+  <si>
+    <t>NXJ80</t>
+  </si>
+  <si>
+    <t>NXK80</t>
+  </si>
+  <si>
+    <t>NXA80</t>
+  </si>
+  <si>
+    <t>NXJ90</t>
+  </si>
+  <si>
+    <t>NXK90</t>
+  </si>
+  <si>
+    <t>NXA90</t>
+  </si>
+  <si>
+    <t>NXJ100</t>
+  </si>
+  <si>
+    <t>NXK100</t>
+  </si>
+  <si>
+    <t>NXC100</t>
+  </si>
+  <si>
+    <t>NXD100</t>
+  </si>
+  <si>
+    <t>NXB120</t>
+  </si>
+  <si>
+    <t>NXD120</t>
+  </si>
+  <si>
+    <t>NXE120</t>
+  </si>
+  <si>
+    <t>NXB140</t>
+  </si>
+  <si>
+    <t>NXC140</t>
+  </si>
+  <si>
+    <t>NXE140</t>
+  </si>
+  <si>
+    <t>NXF140</t>
+  </si>
+  <si>
+    <t>NXC150</t>
+  </si>
+  <si>
+    <t>NXD150</t>
+  </si>
+  <si>
+    <t>NXF150</t>
+  </si>
+  <si>
+    <t>NXG150</t>
+  </si>
+  <si>
+    <t>NXD200</t>
+  </si>
+  <si>
+    <t>NXE200</t>
+  </si>
+  <si>
+    <t>NXG200</t>
+  </si>
+  <si>
+    <t>NXH200</t>
+  </si>
+  <si>
+    <t>NXE250</t>
+  </si>
+  <si>
+    <t>NXF250</t>
+  </si>
+  <si>
+    <t>NXH250</t>
+  </si>
+  <si>
+    <t>NXI250</t>
+  </si>
+  <si>
+    <t>NXF280</t>
+  </si>
+  <si>
+    <t>NXG280</t>
+  </si>
+  <si>
+    <t>NXI280</t>
+  </si>
+  <si>
+    <t>NXG300</t>
+  </si>
+  <si>
+    <t>NXI300</t>
+  </si>
+  <si>
+    <t>NXH320</t>
+  </si>
+  <si>
+    <t>NXI320</t>
+  </si>
+  <si>
+    <t>NXG250*</t>
+  </si>
+  <si>
+    <t>NXH280*</t>
+  </si>
+  <si>
     <t>CAL00001</t>
   </si>
   <si>
@@ -384,205 +576,16 @@
     <t>PTW 30013 5122</t>
   </si>
   <si>
+    <t>Duncan Butler</t>
+  </si>
+  <si>
+    <t>Calibration No: CAL00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06 Oct 2021 </t>
+  </si>
+  <si>
     <t>12 Feb 2021 to 12 Feb 2021</t>
-  </si>
-  <si>
-    <t>Duncan Butler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 Oct 2021 </t>
-  </si>
-  <si>
-    <t>(-250) on the guard electrode Positive (Central Electrode Negative)</t>
-  </si>
-  <si>
-    <t>NXA50</t>
-  </si>
-  <si>
-    <t>NXA70</t>
-  </si>
-  <si>
-    <t>NXB100</t>
-  </si>
-  <si>
-    <t>NXC120</t>
-  </si>
-  <si>
-    <t>NXD140</t>
-  </si>
-  <si>
-    <t>NXE150</t>
-  </si>
-  <si>
-    <t>NXF200</t>
-  </si>
-  <si>
-    <t>NXG250</t>
-  </si>
-  <si>
-    <t>NXH280</t>
-  </si>
-  <si>
-    <t>NXH300</t>
-  </si>
-  <si>
-    <t>NXH300*</t>
-  </si>
-  <si>
-    <t>NXJ40</t>
-  </si>
-  <si>
-    <t>NXK40</t>
-  </si>
-  <si>
-    <t>NXA40</t>
-  </si>
-  <si>
-    <t>NXJ50</t>
-  </si>
-  <si>
-    <t>NXK50</t>
-  </si>
-  <si>
-    <t>NXB50</t>
-  </si>
-  <si>
-    <t>NXJ60</t>
-  </si>
-  <si>
-    <t>NXK60</t>
-  </si>
-  <si>
-    <t>NXA60</t>
-  </si>
-  <si>
-    <t>NXJ70</t>
-  </si>
-  <si>
-    <t>NXK70</t>
-  </si>
-  <si>
-    <t>NXB70</t>
-  </si>
-  <si>
-    <t>NXC70</t>
-  </si>
-  <si>
-    <t>NXJ80</t>
-  </si>
-  <si>
-    <t>NXK80</t>
-  </si>
-  <si>
-    <t>NXA80</t>
-  </si>
-  <si>
-    <t>NXJ90</t>
-  </si>
-  <si>
-    <t>NXK90</t>
-  </si>
-  <si>
-    <t>NXA90</t>
-  </si>
-  <si>
-    <t>NXJ100</t>
-  </si>
-  <si>
-    <t>NXK100</t>
-  </si>
-  <si>
-    <t>NXC100</t>
-  </si>
-  <si>
-    <t>NXD100</t>
-  </si>
-  <si>
-    <t>NXB120</t>
-  </si>
-  <si>
-    <t>NXD120</t>
-  </si>
-  <si>
-    <t>NXE120</t>
-  </si>
-  <si>
-    <t>NXB140</t>
-  </si>
-  <si>
-    <t>NXC140</t>
-  </si>
-  <si>
-    <t>NXE140</t>
-  </si>
-  <si>
-    <t>NXF140</t>
-  </si>
-  <si>
-    <t>NXC150</t>
-  </si>
-  <si>
-    <t>NXD150</t>
-  </si>
-  <si>
-    <t>NXF150</t>
-  </si>
-  <si>
-    <t>NXG150</t>
-  </si>
-  <si>
-    <t>NXD200</t>
-  </si>
-  <si>
-    <t>NXE200</t>
-  </si>
-  <si>
-    <t>NXG200</t>
-  </si>
-  <si>
-    <t>NXH200</t>
-  </si>
-  <si>
-    <t>NXE250</t>
-  </si>
-  <si>
-    <t>NXF250</t>
-  </si>
-  <si>
-    <t>NXH250</t>
-  </si>
-  <si>
-    <t>NXI250</t>
-  </si>
-  <si>
-    <t>NXF280</t>
-  </si>
-  <si>
-    <t>NXG280</t>
-  </si>
-  <si>
-    <t>NXI280</t>
-  </si>
-  <si>
-    <t>NXG300</t>
-  </si>
-  <si>
-    <t>NXI300</t>
-  </si>
-  <si>
-    <t>NXH320</t>
-  </si>
-  <si>
-    <t>NXI320</t>
-  </si>
-  <si>
-    <t>NXG250*</t>
-  </si>
-  <si>
-    <t>NXH280*</t>
-  </si>
-  <si>
-    <t>Calibration No: CAL00001</t>
   </si>
 </sst>
 </file>
@@ -2137,8 +2140,8 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
       <xdr:row>240</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
@@ -2147,7 +2150,7 @@
         <xdr:cNvPr id="4" name="kVp">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AC52595-D671-4208-B415-8AD42483C067}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{334EA707-5F45-464C-A5DF-EC16D2BBFCCF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2156,13 +2159,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2170,7 +2167,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="46413421"/>
-          <a:ext cx="5629910" cy="3352800"/>
+          <a:ext cx="5715000" cy="3352800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2187,17 +2184,17 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>269</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="Al">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F14F04CD-06B6-4DBD-B5B3-F7C2FD711B05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75CDF684-ED7F-476C-AEF5-BFB1A7E29FBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2206,13 +2203,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2220,7 +2211,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="51267361"/>
-          <a:ext cx="5629910" cy="3539490"/>
+          <a:ext cx="5715000" cy="3352800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2233,21 +2224,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>275</xdr:row>
-      <xdr:rowOff>4</xdr:rowOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>167638</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>296</xdr:row>
-      <xdr:rowOff>19054</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>294</xdr:row>
+      <xdr:rowOff>167638</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="Cu">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46C3535F-2CE3-4597-85E6-66D253B38A93}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{078B7652-5463-44E3-BAA6-B27FBE62A48A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2256,21 +2247,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="55801264"/>
-          <a:ext cx="5629910" cy="3539490"/>
+          <a:off x="0" y="55801258"/>
+          <a:ext cx="5715000" cy="3352800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2606,8 +2591,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:X308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q122" sqref="Q122"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Z123" sqref="Z123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
@@ -2796,7 +2781,7 @@
       <c r="R13" s="48"/>
       <c r="S13" s="48"/>
       <c r="T13" s="49" t="s">
-        <v>106</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="14.1" customHeight="1">
@@ -2924,7 +2909,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="50" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="H20" s="51"/>
       <c r="I20" s="51"/>
@@ -2947,7 +2932,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="50" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="H21" s="51"/>
       <c r="I21" s="51"/>
@@ -2970,7 +2955,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="50" t="s">
-        <v>110</v>
+        <v>173</v>
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="51"/>
@@ -3037,7 +3022,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="51" t="s">
-        <v>111</v>
+        <v>174</v>
       </c>
       <c r="H25" s="51"/>
       <c r="I25" s="51"/>
@@ -3083,7 +3068,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="51" t="s">
-        <v>112</v>
+        <v>178</v>
       </c>
       <c r="H27" s="51"/>
       <c r="I27" s="51"/>
@@ -3176,7 +3161,7 @@
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="52" t="s">
-        <v>113</v>
+        <v>175</v>
       </c>
       <c r="H31" s="51"/>
       <c r="I31" s="51"/>
@@ -3201,7 +3186,7 @@
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="51" t="s">
-        <v>113</v>
+        <v>175</v>
       </c>
       <c r="H32" s="51"/>
       <c r="I32" s="51"/>
@@ -3226,7 +3211,7 @@
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="52" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="H33" s="51"/>
       <c r="I33" s="51"/>
@@ -3552,7 +3537,7 @@
     </row>
     <row r="57" spans="1:20" ht="14.1" customHeight="1">
       <c r="A57" s="53" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B57" s="54"/>
       <c r="C57" s="54"/>
@@ -3562,7 +3547,7 @@
       <c r="G57" s="18"/>
       <c r="H57" s="18"/>
       <c r="I57" s="55" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J57" s="54"/>
       <c r="K57" s="18"/>
@@ -4195,7 +4180,7 @@
       <c r="D110" s="26"/>
       <c r="E110" s="26"/>
       <c r="G110" s="50" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="H110" s="48"/>
       <c r="I110" s="48"/>
@@ -4217,7 +4202,7 @@
       <c r="D111" s="26"/>
       <c r="E111" s="26"/>
       <c r="G111" s="57" t="s">
-        <v>111</v>
+        <v>174</v>
       </c>
       <c r="H111" s="48"/>
       <c r="I111" s="48"/>
@@ -4261,7 +4246,7 @@
       <c r="D113" s="26"/>
       <c r="E113" s="26"/>
       <c r="G113" s="58" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="H113" s="48"/>
       <c r="I113" s="48"/>
@@ -4470,7 +4455,7 @@
       <c r="D123" s="26"/>
       <c r="E123" s="26"/>
       <c r="G123" s="48" t="s">
-        <v>112</v>
+        <v>178</v>
       </c>
       <c r="H123" s="48"/>
       <c r="I123" s="48"/>
@@ -4628,7 +4613,7 @@
     </row>
     <row r="129" spans="1:20" ht="20.25" customHeight="1">
       <c r="A129" s="122" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B129" s="65"/>
       <c r="C129" s="122">
@@ -4668,7 +4653,7 @@
     </row>
     <row r="130" spans="1:20" ht="20.25" customHeight="1">
       <c r="A130" s="125" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B130" s="71"/>
       <c r="C130" s="125">
@@ -4708,7 +4693,7 @@
     </row>
     <row r="131" spans="1:20" ht="20.25" customHeight="1">
       <c r="A131" s="132" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B131" s="71"/>
       <c r="C131" s="132">
@@ -4748,7 +4733,7 @@
     </row>
     <row r="132" spans="1:20" ht="20.25" customHeight="1">
       <c r="A132" s="125" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B132" s="71"/>
       <c r="C132" s="125">
@@ -4788,7 +4773,7 @@
     </row>
     <row r="133" spans="1:20" ht="20.25" customHeight="1">
       <c r="A133" s="132" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B133" s="71"/>
       <c r="C133" s="132">
@@ -4828,7 +4813,7 @@
     </row>
     <row r="134" spans="1:20" ht="20.25" customHeight="1">
       <c r="A134" s="125" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B134" s="71"/>
       <c r="C134" s="125">
@@ -4868,7 +4853,7 @@
     </row>
     <row r="135" spans="1:20" ht="20.25" customHeight="1">
       <c r="A135" s="132" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B135" s="71"/>
       <c r="C135" s="132">
@@ -4908,7 +4893,7 @@
     </row>
     <row r="136" spans="1:20" ht="20.25" customHeight="1">
       <c r="A136" s="125" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B136" s="71"/>
       <c r="C136" s="125">
@@ -4948,7 +4933,7 @@
     </row>
     <row r="137" spans="1:20" ht="20.25" customHeight="1">
       <c r="A137" s="132" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B137" s="71"/>
       <c r="C137" s="132">
@@ -4988,7 +4973,7 @@
     </row>
     <row r="138" spans="1:20" ht="20.25" customHeight="1">
       <c r="A138" s="136" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B138" s="80"/>
       <c r="C138" s="125">
@@ -5028,7 +5013,7 @@
     </row>
     <row r="139" spans="1:20" ht="14.1" customHeight="1">
       <c r="A139" s="140" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B139" s="111"/>
       <c r="C139" s="140">
@@ -5142,7 +5127,7 @@
       <c r="J143" s="26"/>
       <c r="K143" s="26"/>
       <c r="L143" s="59" t="s">
-        <v>108</v>
+        <v>171</v>
       </c>
       <c r="M143" s="59"/>
       <c r="N143" s="59"/>
@@ -5314,7 +5299,7 @@
     </row>
     <row r="151" spans="1:21" ht="14.25" customHeight="1">
       <c r="A151" s="84" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B151" s="65"/>
       <c r="C151" s="84">
@@ -5352,7 +5337,7 @@
     </row>
     <row r="152" spans="1:21" ht="14.25" customHeight="1">
       <c r="A152" s="92" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B152" s="71"/>
       <c r="C152" s="92">
@@ -5390,7 +5375,7 @@
     </row>
     <row r="153" spans="1:21" ht="14.25" customHeight="1">
       <c r="A153" s="95" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B153" s="80"/>
       <c r="C153" s="95">
@@ -5430,7 +5415,7 @@
     </row>
     <row r="154" spans="1:21" ht="14.25" customHeight="1">
       <c r="A154" s="94" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B154" s="65"/>
       <c r="C154" s="94">
@@ -5468,7 +5453,7 @@
     </row>
     <row r="155" spans="1:21" ht="14.25" customHeight="1">
       <c r="A155" s="70" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B155" s="71"/>
       <c r="C155" s="70">
@@ -5506,7 +5491,7 @@
     </row>
     <row r="156" spans="1:21" ht="14.25" customHeight="1">
       <c r="A156" s="92" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B156" s="71"/>
       <c r="C156" s="92">
@@ -5546,7 +5531,7 @@
     </row>
     <row r="157" spans="1:21" ht="14.25" customHeight="1">
       <c r="A157" s="95" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B157" s="80"/>
       <c r="C157" s="95">
@@ -5586,7 +5571,7 @@
     </row>
     <row r="158" spans="1:21" ht="14.25" customHeight="1">
       <c r="A158" s="94" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B158" s="65"/>
       <c r="C158" s="94">
@@ -5624,7 +5609,7 @@
     </row>
     <row r="159" spans="1:21" ht="14.25" customHeight="1">
       <c r="A159" s="70" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B159" s="71"/>
       <c r="C159" s="70">
@@ -5662,7 +5647,7 @@
     </row>
     <row r="160" spans="1:21" ht="14.25" customHeight="1">
       <c r="A160" s="79" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B160" s="80"/>
       <c r="C160" s="79">
@@ -5702,7 +5687,7 @@
     </row>
     <row r="161" spans="1:20" ht="14.25" customHeight="1">
       <c r="A161" s="84" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B161" s="65"/>
       <c r="C161" s="84">
@@ -5740,7 +5725,7 @@
     </row>
     <row r="162" spans="1:20" ht="14.25" customHeight="1">
       <c r="A162" s="92" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B162" s="71"/>
       <c r="C162" s="92">
@@ -5778,7 +5763,7 @@
     </row>
     <row r="163" spans="1:20" ht="14.25" customHeight="1">
       <c r="A163" s="70" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B163" s="71"/>
       <c r="C163" s="70">
@@ -5818,7 +5803,7 @@
     </row>
     <row r="164" spans="1:20" ht="14.25" customHeight="1">
       <c r="A164" s="92" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B164" s="71"/>
       <c r="C164" s="92">
@@ -5858,7 +5843,7 @@
     </row>
     <row r="165" spans="1:20" ht="14.25" customHeight="1">
       <c r="A165" s="70" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B165" s="71"/>
       <c r="C165" s="70">
@@ -5898,7 +5883,7 @@
     </row>
     <row r="166" spans="1:20" ht="14.25" customHeight="1">
       <c r="A166" s="94" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B166" s="65"/>
       <c r="C166" s="94">
@@ -5936,7 +5921,7 @@
     </row>
     <row r="167" spans="1:20" ht="14.25" customHeight="1">
       <c r="A167" s="70" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B167" s="71"/>
       <c r="C167" s="70">
@@ -5974,7 +5959,7 @@
     </row>
     <row r="168" spans="1:20" ht="14.25" customHeight="1">
       <c r="A168" s="79" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B168" s="80"/>
       <c r="C168" s="79">
@@ -6014,7 +5999,7 @@
     </row>
     <row r="169" spans="1:20" ht="14.25" customHeight="1">
       <c r="A169" s="84" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B169" s="65"/>
       <c r="C169" s="84">
@@ -6052,7 +6037,7 @@
     </row>
     <row r="170" spans="1:20" ht="14.25" customHeight="1">
       <c r="A170" s="92" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B170" s="71"/>
       <c r="C170" s="92">
@@ -6090,7 +6075,7 @@
     </row>
     <row r="171" spans="1:20" ht="14.25" customHeight="1">
       <c r="A171" s="70" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B171" s="71"/>
       <c r="C171" s="70">
@@ -6130,7 +6115,7 @@
     </row>
     <row r="172" spans="1:20" ht="14.25" customHeight="1">
       <c r="A172" s="94" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B172" s="65"/>
       <c r="C172" s="94">
@@ -6168,7 +6153,7 @@
     </row>
     <row r="173" spans="1:20" ht="14.25" customHeight="1">
       <c r="A173" s="70" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B173" s="71"/>
       <c r="C173" s="70">
@@ -6206,7 +6191,7 @@
     </row>
     <row r="174" spans="1:20" ht="14.25" customHeight="1">
       <c r="A174" s="92" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B174" s="71"/>
       <c r="C174" s="92">
@@ -6246,7 +6231,7 @@
     </row>
     <row r="175" spans="1:20" ht="14.25" customHeight="1">
       <c r="A175" s="70" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B175" s="71"/>
       <c r="C175" s="70">
@@ -6286,7 +6271,7 @@
     </row>
     <row r="176" spans="1:20" ht="14.25" customHeight="1">
       <c r="A176" s="79" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B176" s="80"/>
       <c r="C176" s="79">
@@ -6326,7 +6311,7 @@
     </row>
     <row r="177" spans="1:20" ht="14.25" customHeight="1">
       <c r="A177" s="70" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B177" s="71"/>
       <c r="C177" s="70">
@@ -6366,7 +6351,7 @@
     </row>
     <row r="178" spans="1:20" ht="14.25" customHeight="1">
       <c r="A178" s="92" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B178" s="71"/>
       <c r="C178" s="92">
@@ -6406,7 +6391,7 @@
     </row>
     <row r="179" spans="1:20" ht="14.25" customHeight="1">
       <c r="A179" s="70" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B179" s="71"/>
       <c r="C179" s="70">
@@ -6446,7 +6431,7 @@
     </row>
     <row r="180" spans="1:20" ht="14.25" customHeight="1">
       <c r="A180" s="79" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B180" s="80"/>
       <c r="C180" s="79">
@@ -6488,7 +6473,7 @@
     </row>
     <row r="181" spans="1:20" ht="14.25" customHeight="1">
       <c r="A181" s="84" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B181" s="65"/>
       <c r="C181" s="84">
@@ -6528,7 +6513,7 @@
     </row>
     <row r="182" spans="1:20" ht="14.25" customHeight="1">
       <c r="A182" s="92" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B182" s="71"/>
       <c r="C182" s="92">
@@ -6568,7 +6553,7 @@
     </row>
     <row r="183" spans="1:20" ht="14.25" customHeight="1">
       <c r="A183" s="70" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B183" s="71"/>
       <c r="C183" s="70">
@@ -6608,7 +6593,7 @@
     </row>
     <row r="184" spans="1:20" ht="14.25" customHeight="1">
       <c r="A184" s="92" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B184" s="71"/>
       <c r="C184" s="92">
@@ -6648,7 +6633,7 @@
     </row>
     <row r="185" spans="1:20" ht="14.25" customHeight="1">
       <c r="A185" s="95" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B185" s="80"/>
       <c r="C185" s="95">
@@ -6688,7 +6673,7 @@
     </row>
     <row r="186" spans="1:20" ht="14.25" customHeight="1">
       <c r="A186" s="94" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B186" s="65"/>
       <c r="C186" s="94">
@@ -6728,7 +6713,7 @@
     </row>
     <row r="187" spans="1:20" ht="14.25" customHeight="1">
       <c r="A187" s="70" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B187" s="71"/>
       <c r="C187" s="70">
@@ -6768,7 +6753,7 @@
     </row>
     <row r="188" spans="1:20" ht="14.25" customHeight="1">
       <c r="A188" s="92" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B188" s="71"/>
       <c r="C188" s="92">
@@ -6808,7 +6793,7 @@
     </row>
     <row r="189" spans="1:20" ht="14.1" customHeight="1">
       <c r="A189" s="70" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B189" s="71"/>
       <c r="C189" s="70">
@@ -6848,7 +6833,7 @@
     </row>
     <row r="190" spans="1:20" ht="16.5" customHeight="1">
       <c r="A190" s="79" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B190" s="80"/>
       <c r="C190" s="79">
@@ -7031,7 +7016,7 @@
     </row>
     <row r="198" spans="1:20" ht="14.25" customHeight="1">
       <c r="A198" s="84" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B198" s="65"/>
       <c r="C198" s="84">
@@ -7071,7 +7056,7 @@
     </row>
     <row r="199" spans="1:20" ht="14.25" customHeight="1">
       <c r="A199" s="92" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B199" s="71"/>
       <c r="C199" s="92">
@@ -7111,7 +7096,7 @@
     </row>
     <row r="200" spans="1:20" ht="14.25" customHeight="1">
       <c r="A200" s="70" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B200" s="71"/>
       <c r="C200" s="70">
@@ -7151,7 +7136,7 @@
     </row>
     <row r="201" spans="1:20" ht="14.25" customHeight="1">
       <c r="A201" s="92" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B201" s="71"/>
       <c r="C201" s="92">
@@ -7191,7 +7176,7 @@
     </row>
     <row r="202" spans="1:20" ht="14.25" customHeight="1">
       <c r="A202" s="95" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B202" s="80"/>
       <c r="C202" s="95">
@@ -7231,7 +7216,7 @@
     </row>
     <row r="203" spans="1:20" ht="14.25" customHeight="1">
       <c r="A203" s="94" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B203" s="65"/>
       <c r="C203" s="94">
@@ -7271,7 +7256,7 @@
     </row>
     <row r="204" spans="1:20" ht="14.25" customHeight="1">
       <c r="A204" s="70" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B204" s="71"/>
       <c r="C204" s="70">
@@ -7311,7 +7296,7 @@
     </row>
     <row r="205" spans="1:20" ht="14.25" customHeight="1">
       <c r="A205" s="92" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B205" s="71"/>
       <c r="C205" s="92">
@@ -7351,7 +7336,7 @@
     </row>
     <row r="206" spans="1:20" ht="14.25" customHeight="1">
       <c r="A206" s="70" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B206" s="71"/>
       <c r="C206" s="70">
@@ -7391,7 +7376,7 @@
     </row>
     <row r="207" spans="1:20" ht="14.25" customHeight="1">
       <c r="A207" s="79" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B207" s="80"/>
       <c r="C207" s="79">
@@ -7431,7 +7416,7 @@
     </row>
     <row r="208" spans="1:20" ht="14.25" customHeight="1">
       <c r="A208" s="70" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B208" s="71"/>
       <c r="C208" s="70">
@@ -7471,7 +7456,7 @@
     </row>
     <row r="209" spans="1:20" ht="14.25" customHeight="1">
       <c r="A209" s="92" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B209" s="71"/>
       <c r="C209" s="92">
@@ -7511,7 +7496,7 @@
     </row>
     <row r="210" spans="1:20" ht="14.25" customHeight="1">
       <c r="A210" s="70" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B210" s="71"/>
       <c r="C210" s="70">
@@ -7551,7 +7536,7 @@
     </row>
     <row r="211" spans="1:20" ht="14.25" customHeight="1">
       <c r="A211" s="79" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B211" s="80"/>
       <c r="C211" s="79">
@@ -7591,7 +7576,7 @@
     </row>
     <row r="212" spans="1:20" ht="14.25" customHeight="1">
       <c r="A212" s="84" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B212" s="65"/>
       <c r="C212" s="84">
@@ -7631,7 +7616,7 @@
     </row>
     <row r="213" spans="1:20" ht="14.25" customHeight="1">
       <c r="A213" s="92" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B213" s="71"/>
       <c r="C213" s="92">
@@ -7671,7 +7656,7 @@
     </row>
     <row r="214" spans="1:20" ht="14.25" customHeight="1">
       <c r="A214" s="70" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B214" s="71"/>
       <c r="C214" s="70">
@@ -7711,7 +7696,7 @@
     </row>
     <row r="215" spans="1:20" ht="14.25" customHeight="1">
       <c r="A215" s="94" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B215" s="65"/>
       <c r="C215" s="94">
@@ -7751,7 +7736,7 @@
     </row>
     <row r="216" spans="1:20" ht="14.25" customHeight="1">
       <c r="A216" s="70" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B216" s="71"/>
       <c r="C216" s="70">
@@ -7791,7 +7776,7 @@
     </row>
     <row r="217" spans="1:20" ht="15" customHeight="1">
       <c r="A217" s="145" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B217" s="111"/>
       <c r="C217" s="145">
@@ -7831,7 +7816,7 @@
     </row>
     <row r="218" spans="1:20" ht="15" customHeight="1">
       <c r="A218" s="164" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B218" s="111"/>
       <c r="C218" s="164">
@@ -7871,7 +7856,7 @@
     </row>
     <row r="219" spans="1:20" ht="15" customHeight="1">
       <c r="A219" s="145" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B219" s="111"/>
       <c r="C219" s="145">

</xml_diff>

<commit_message>
add high resolution on pdf chart
</commit_message>
<xml_diff>
--- a/app/core/testing.xlsx
+++ b/app/core/testing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DC-Boxjelly\app\core\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0CDB7D-1BF1-4C96-9819-E362409E3E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="990" windowWidth="29040" windowHeight="15840" tabRatio="807" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="990" windowWidth="29040" windowHeight="15840" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="MEXReport" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
     <definedName name="REPORT_Dir">#REF!</definedName>
     <definedName name="THIS_Dir">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="188">
   <si>
     <t>Primary Standards Dosimetry Laboratory,  Medical Radiation Services</t>
   </si>
@@ -366,231 +365,340 @@
     <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
+    <t>PTW 30013 5122</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">06 Oct 2021 </t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calibrated by: ClientA_Name</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duncan Butler</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>(-250) on the guard electrode Positive (Central Electrode Negative)</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXA50</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXC70</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXD200</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXF280</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
     <t>CAL00001</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>ClientA_Name</t>
-  </si>
-  <si>
-    <t>Calibrated by: ClientA_Name</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClientA_Name</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>200 Street Name</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>Suburb NSW 2020</t>
-  </si>
-  <si>
-    <t>PTW 30013 5122</t>
-  </si>
-  <si>
-    <t>12 Feb 2021 to 12 Feb 2021</t>
-  </si>
-  <si>
-    <t>Duncan Butler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 Oct 2021 </t>
-  </si>
-  <si>
-    <t>(-250) on the guard electrode Positive (Central Electrode Negative)</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>12 Feb 2021 to 01 Mar 2021</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>12 Feb 2021 to 01 Mar 2021</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXA70</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXB100</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXC120</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXD140</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXE150</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXF200</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXG250</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXH280</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXH300</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXH300*</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXJ40</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXK40</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXA40</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXJ50</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXK50</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>NXA50</t>
-  </si>
-  <si>
-    <t>NXA70</t>
-  </si>
-  <si>
-    <t>NXB100</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXB50</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXJ60</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXK60</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXA60</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXJ70</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXK70</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXB70</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXJ80</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXK80</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXA80</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXJ90</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXK90</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXA90</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXJ100</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXK100</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXC100</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXD100</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXB120</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>NXC120</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXD120</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXE120</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXB140</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXC140</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>NXD140</t>
-  </si>
-  <si>
-    <t>NXE150</t>
-  </si>
-  <si>
-    <t>NXF200</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXE140</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXF140</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXC150</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXD150</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXF150</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXG150</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXE200</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXG200</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXH200</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXE250</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXF250</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>NXG250</t>
-  </si>
-  <si>
-    <t>NXH280</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXH250</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXI250</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXG280</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXI280</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXG300</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>NXH300</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXI300</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXH320</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXI320</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXG250*</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>NXH280*</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>NXH300*</t>
-  </si>
-  <si>
-    <t>NXJ40</t>
-  </si>
-  <si>
-    <t>NXK40</t>
-  </si>
-  <si>
-    <t>NXA40</t>
-  </si>
-  <si>
-    <t>NXJ50</t>
-  </si>
-  <si>
-    <t>NXK50</t>
-  </si>
-  <si>
-    <t>NXB50</t>
-  </si>
-  <si>
-    <t>NXJ60</t>
-  </si>
-  <si>
-    <t>NXK60</t>
-  </si>
-  <si>
-    <t>NXA60</t>
-  </si>
-  <si>
-    <t>NXJ70</t>
-  </si>
-  <si>
-    <t>NXK70</t>
-  </si>
-  <si>
-    <t>NXB70</t>
-  </si>
-  <si>
-    <t>NXC70</t>
-  </si>
-  <si>
-    <t>NXJ80</t>
-  </si>
-  <si>
-    <t>NXK80</t>
-  </si>
-  <si>
-    <t>NXA80</t>
-  </si>
-  <si>
-    <t>NXJ90</t>
-  </si>
-  <si>
-    <t>NXK90</t>
-  </si>
-  <si>
-    <t>NXA90</t>
-  </si>
-  <si>
-    <t>NXJ100</t>
-  </si>
-  <si>
-    <t>NXK100</t>
-  </si>
-  <si>
-    <t>NXC100</t>
-  </si>
-  <si>
-    <t>NXD100</t>
-  </si>
-  <si>
-    <t>NXB120</t>
-  </si>
-  <si>
-    <t>NXD120</t>
-  </si>
-  <si>
-    <t>NXE120</t>
-  </si>
-  <si>
-    <t>NXB140</t>
-  </si>
-  <si>
-    <t>NXC140</t>
-  </si>
-  <si>
-    <t>NXE140</t>
-  </si>
-  <si>
-    <t>NXF140</t>
-  </si>
-  <si>
-    <t>NXC150</t>
-  </si>
-  <si>
-    <t>NXD150</t>
-  </si>
-  <si>
-    <t>NXF150</t>
-  </si>
-  <si>
-    <t>NXG150</t>
-  </si>
-  <si>
-    <t>NXD200</t>
-  </si>
-  <si>
-    <t>NXE200</t>
-  </si>
-  <si>
-    <t>NXG200</t>
-  </si>
-  <si>
-    <t>NXH200</t>
-  </si>
-  <si>
-    <t>NXE250</t>
-  </si>
-  <si>
-    <t>NXF250</t>
-  </si>
-  <si>
-    <t>NXH250</t>
-  </si>
-  <si>
-    <t>NXI250</t>
-  </si>
-  <si>
-    <t>NXF280</t>
-  </si>
-  <si>
-    <t>NXG280</t>
-  </si>
-  <si>
-    <t>NXI280</t>
-  </si>
-  <si>
-    <t>NXG300</t>
-  </si>
-  <si>
-    <t>NXI300</t>
-  </si>
-  <si>
-    <t>NXH320</t>
-  </si>
-  <si>
-    <t>NXI320</t>
-  </si>
-  <si>
-    <t>NXG250*</t>
-  </si>
-  <si>
-    <t>NXH280*</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
   <si>
     <t>Calibration No: CAL00001</t>
+    <phoneticPr fontId="42" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calibration No: CAL00001</t>
+    <phoneticPr fontId="42" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
   <fonts count="43">
     <font>
@@ -661,21 +769,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -683,7 +791,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -691,7 +799,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -699,14 +807,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -714,7 +822,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -722,7 +830,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -730,28 +838,28 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -759,7 +867,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -767,14 +875,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -813,7 +921,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1520,14 +1628,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1542,7 +1650,7 @@
     <xf numFmtId="1" fontId="41" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="41" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1557,7 +1665,7 @@
     <xf numFmtId="1" fontId="41" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="41" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1592,7 +1700,7 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="33" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="33" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -1600,7 +1708,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1612,7 +1720,7 @@
     <xf numFmtId="1" fontId="41" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="41" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="41" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1631,14 +1739,14 @@
     <xf numFmtId="1" fontId="41" fillId="33" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="33" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="41" fillId="33" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="41" fillId="34" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1653,17 +1761,17 @@
     <xf numFmtId="1" fontId="41" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="41" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="33" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="33" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1675,7 +1783,7 @@
     <xf numFmtId="1" fontId="41" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="41" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1690,7 +1798,7 @@
     <xf numFmtId="1" fontId="41" fillId="33" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="33" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="41" fillId="33" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="41" fillId="34" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1700,7 +1808,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1712,13 +1820,13 @@
     <xf numFmtId="1" fontId="41" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="41" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="41" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1733,13 +1841,13 @@
     <xf numFmtId="2" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="28" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1748,13 +1856,13 @@
     <xf numFmtId="0" fontId="5" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="28" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="28" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1766,7 +1874,7 @@
     <xf numFmtId="2" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1775,7 +1883,7 @@
     <xf numFmtId="2" fontId="5" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1809,7 +1917,7 @@
     <xf numFmtId="2" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="28" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="28" fillId="34" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1817,52 +1925,52 @@
     </xf>
   </cellXfs>
   <cellStyles count="46">
-    <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Calculation 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Check Cell 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Good 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Heading 1 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Heading 2 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Heading 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Heading 4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Input 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Neutral 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 4" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 6" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Output 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Total 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Warning Text 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="1"/>
+    <cellStyle name="20% - Accent2 2" xfId="2"/>
+    <cellStyle name="20% - Accent3 2" xfId="3"/>
+    <cellStyle name="20% - Accent4 2" xfId="4"/>
+    <cellStyle name="20% - Accent5 2" xfId="5"/>
+    <cellStyle name="20% - Accent6 2" xfId="6"/>
+    <cellStyle name="40% - Accent1 2" xfId="7"/>
+    <cellStyle name="40% - Accent2 2" xfId="8"/>
+    <cellStyle name="40% - Accent3 2" xfId="9"/>
+    <cellStyle name="40% - Accent4 2" xfId="10"/>
+    <cellStyle name="40% - Accent5 2" xfId="11"/>
+    <cellStyle name="40% - Accent6 2" xfId="12"/>
+    <cellStyle name="60% - Accent1 2" xfId="13"/>
+    <cellStyle name="60% - Accent2 2" xfId="14"/>
+    <cellStyle name="60% - Accent3 2" xfId="15"/>
+    <cellStyle name="60% - Accent4 2" xfId="16"/>
+    <cellStyle name="60% - Accent5 2" xfId="17"/>
+    <cellStyle name="60% - Accent6 2" xfId="18"/>
+    <cellStyle name="Accent1 2" xfId="19"/>
+    <cellStyle name="Accent2 2" xfId="20"/>
+    <cellStyle name="Accent3 2" xfId="21"/>
+    <cellStyle name="Accent4 2" xfId="22"/>
+    <cellStyle name="Accent5 2" xfId="23"/>
+    <cellStyle name="Accent6 2" xfId="24"/>
+    <cellStyle name="Bad 2" xfId="25"/>
+    <cellStyle name="Calculation 2" xfId="26"/>
+    <cellStyle name="Check Cell 2" xfId="27"/>
+    <cellStyle name="Explanatory Text 2" xfId="28"/>
+    <cellStyle name="Good 2" xfId="29"/>
+    <cellStyle name="Heading 1 2" xfId="30"/>
+    <cellStyle name="Heading 2 2" xfId="31"/>
+    <cellStyle name="Heading 3 2" xfId="32"/>
+    <cellStyle name="Heading 4 2" xfId="33"/>
+    <cellStyle name="Input 2" xfId="34"/>
+    <cellStyle name="Linked Cell 2" xfId="35"/>
+    <cellStyle name="Neutral 2" xfId="36"/>
+    <cellStyle name="Normal 2" xfId="37"/>
+    <cellStyle name="Normal 2 2" xfId="38"/>
+    <cellStyle name="Normal 3" xfId="39"/>
+    <cellStyle name="Normal 4" xfId="40"/>
+    <cellStyle name="Normal 6" xfId="41"/>
+    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="Output 2" xfId="43"/>
+    <cellStyle name="Total 2" xfId="44"/>
+    <cellStyle name="Warning Text 2" xfId="45"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2133,30 +2241,24 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>222</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:row>223</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>273050</xdr:colOff>
       <xdr:row>240</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="kVp">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{891459CC-9ADB-49A2-800E-D3951F7DFE76}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="kVp"/>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2169,8 +2271,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="45506639"/>
-          <a:ext cx="5629910" cy="3352800"/>
+          <a:off x="0" y="46739175"/>
+          <a:ext cx="5454650" cy="3352800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2184,23 +2286,17 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>247</xdr:row>
-      <xdr:rowOff>167639</xdr:rowOff>
+      <xdr:rowOff>158117</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>273050</xdr:colOff>
       <xdr:row>269</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>19052</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Al">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C3FBC32-C405-4C16-A122-44B67A624952}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="6" name="Al"/>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -2219,8 +2315,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="50116739"/>
-          <a:ext cx="5629910" cy="3539490"/>
+          <a:off x="0" y="51555017"/>
+          <a:ext cx="5454650" cy="3423285"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2234,23 +2330,17 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>275</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>273050</xdr:colOff>
       <xdr:row>296</xdr:row>
-      <xdr:rowOff>19052</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Cu">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFA46C8B-64BC-460C-B732-4647BF8DA697}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="7" name="Cu"/>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -2269,8 +2359,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="54650642"/>
-          <a:ext cx="5629910" cy="3539490"/>
+          <a:off x="0" y="55940325"/>
+          <a:ext cx="5454650" cy="3419475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2283,7 +2373,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2358,23 +2448,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2410,23 +2483,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2602,7 +2658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:X308"/>
   <sheetViews>
@@ -2610,27 +2666,27 @@
       <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="32" customWidth="1"/>
-    <col min="2" max="2" width="4.33203125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" style="32" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" style="32" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" style="32" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" style="32" customWidth="1"/>
-    <col min="7" max="7" width="4.44140625" style="32" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="4.44140625" style="32" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" style="32" customWidth="1"/>
-    <col min="11" max="11" width="4.44140625" style="32" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" style="32" customWidth="1"/>
-    <col min="13" max="13" width="4.44140625" style="32" customWidth="1"/>
-    <col min="14" max="14" width="5.109375" style="32" customWidth="1"/>
-    <col min="15" max="16" width="4.44140625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="32" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="4.42578125" style="32" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" style="32" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" style="32" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="32" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" style="32" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" style="32" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" style="32" customWidth="1"/>
+    <col min="13" max="13" width="4.42578125" style="32" customWidth="1"/>
+    <col min="14" max="14" width="5.140625" style="32" customWidth="1"/>
+    <col min="15" max="16" width="4.42578125" style="32" customWidth="1"/>
     <col min="17" max="17" width="5" style="32" customWidth="1"/>
-    <col min="18" max="18" width="1.109375" style="32" customWidth="1"/>
-    <col min="19" max="19" width="0.88671875" style="32" customWidth="1"/>
-    <col min="20" max="20" width="4.44140625" style="32" customWidth="1"/>
+    <col min="18" max="18" width="1.140625" style="32" customWidth="1"/>
+    <col min="19" max="19" width="0.85546875" style="32" customWidth="1"/>
+    <col min="20" max="20" width="4.42578125" style="32" customWidth="1"/>
     <col min="21" max="24" width="5" style="32" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2754,7 +2810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15.9" customHeight="1">
+    <row r="12" spans="1:20" ht="15.95" customHeight="1">
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -2775,7 +2831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15.9" customHeight="1">
+    <row r="13" spans="1:20" ht="15.95" customHeight="1">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
@@ -2796,7 +2852,7 @@
       <c r="R13" s="48"/>
       <c r="S13" s="48"/>
       <c r="T13" s="49" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="14.1" customHeight="1">
@@ -2914,7 +2970,7 @@
       <c r="R19" s="26"/>
       <c r="S19" s="26"/>
     </row>
-    <row r="20" spans="1:20" ht="15.9" customHeight="1">
+    <row r="20" spans="1:20" ht="15.95" customHeight="1">
       <c r="A20" s="14" t="s">
         <v>9</v>
       </c>
@@ -2924,7 +2980,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="50" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="H20" s="51"/>
       <c r="I20" s="51"/>
@@ -2939,7 +2995,7 @@
       <c r="R20" s="26"/>
       <c r="S20" s="26"/>
     </row>
-    <row r="21" spans="1:20" ht="15.9" customHeight="1">
+    <row r="21" spans="1:20" ht="15.95" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -2947,7 +3003,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="50" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="H21" s="51"/>
       <c r="I21" s="51"/>
@@ -2962,7 +3018,7 @@
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
     </row>
-    <row r="22" spans="1:20" ht="15.9" customHeight="1">
+    <row r="22" spans="1:20" ht="15.95" customHeight="1">
       <c r="A22" s="14"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -2970,7 +3026,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="50" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="H22" s="51"/>
       <c r="I22" s="51"/>
@@ -2985,7 +3041,7 @@
       <c r="R22" s="26"/>
       <c r="S22" s="26"/>
     </row>
-    <row r="23" spans="1:20" ht="15.9" customHeight="1">
+    <row r="23" spans="1:20" ht="15.95" customHeight="1">
       <c r="A23" s="14"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -3006,7 +3062,7 @@
       <c r="R23" s="26"/>
       <c r="S23" s="26"/>
     </row>
-    <row r="24" spans="1:20" ht="15.9" customHeight="1">
+    <row r="24" spans="1:20" ht="15.95" customHeight="1">
       <c r="A24" s="14"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -3027,7 +3083,7 @@
       <c r="R24" s="26"/>
       <c r="S24" s="26"/>
     </row>
-    <row r="25" spans="1:20" ht="15.9" customHeight="1">
+    <row r="25" spans="1:20" ht="15.95" customHeight="1">
       <c r="A25" s="14" t="s">
         <v>10</v>
       </c>
@@ -3037,7 +3093,7 @@
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="51" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H25" s="51"/>
       <c r="I25" s="51"/>
@@ -3052,7 +3108,7 @@
       <c r="R25" s="26"/>
       <c r="S25" s="26"/>
     </row>
-    <row r="26" spans="1:20" ht="15.9" customHeight="1">
+    <row r="26" spans="1:20" ht="15.95" customHeight="1">
       <c r="A26" s="14"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -3073,7 +3129,7 @@
       <c r="R26" s="26"/>
       <c r="S26" s="26"/>
     </row>
-    <row r="27" spans="1:20" ht="15.9" customHeight="1">
+    <row r="27" spans="1:20" ht="15.95" customHeight="1">
       <c r="A27" s="14" t="s">
         <v>105</v>
       </c>
@@ -3083,7 +3139,7 @@
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="51" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="H27" s="51"/>
       <c r="I27" s="51"/>
@@ -3098,7 +3154,7 @@
       <c r="R27" s="26"/>
       <c r="S27" s="26"/>
     </row>
-    <row r="28" spans="1:20" ht="15.9" customHeight="1">
+    <row r="28" spans="1:20" ht="15.95" customHeight="1">
       <c r="A28" s="14"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -3145,7 +3201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="15.9" customHeight="1">
+    <row r="30" spans="1:20" ht="15.95" customHeight="1">
       <c r="A30" s="14"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3166,7 +3222,7 @@
       <c r="S30" s="26"/>
       <c r="T30" s="62"/>
     </row>
-    <row r="31" spans="1:20" ht="15.9" customHeight="1">
+    <row r="31" spans="1:20" ht="15.95" customHeight="1">
       <c r="A31" s="14" t="s">
         <v>14</v>
       </c>
@@ -3176,7 +3232,7 @@
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="52" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H31" s="51"/>
       <c r="I31" s="51"/>
@@ -3201,7 +3257,7 @@
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="51" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H32" s="51"/>
       <c r="I32" s="51"/>
@@ -3216,7 +3272,7 @@
       <c r="S32" s="26"/>
       <c r="T32" s="62"/>
     </row>
-    <row r="33" spans="1:20" ht="15.9" customHeight="1">
+    <row r="33" spans="1:20" ht="15.95" customHeight="1">
       <c r="A33" s="14" t="s">
         <v>16</v>
       </c>
@@ -3226,7 +3282,7 @@
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="52" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="H33" s="51"/>
       <c r="I33" s="51"/>
@@ -3241,7 +3297,7 @@
       <c r="S33" s="26"/>
       <c r="T33" s="62"/>
     </row>
-    <row r="34" spans="1:20" ht="15.9" customHeight="1">
+    <row r="34" spans="1:20" ht="15.95" customHeight="1">
       <c r="A34" s="14"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3262,7 +3318,7 @@
       <c r="S34" s="26"/>
       <c r="T34" s="62"/>
     </row>
-    <row r="35" spans="1:20" ht="15.9" customHeight="1">
+    <row r="35" spans="1:20" ht="15.95" customHeight="1">
       <c r="A35" s="13" t="s">
         <v>17</v>
       </c>
@@ -3287,7 +3343,7 @@
       <c r="S35" s="26"/>
       <c r="T35" s="62"/>
     </row>
-    <row r="36" spans="1:20" ht="15.9" customHeight="1">
+    <row r="36" spans="1:20" ht="15.95" customHeight="1">
       <c r="A36" s="14" t="s">
         <v>19</v>
       </c>
@@ -3312,7 +3368,7 @@
       <c r="S36" s="26"/>
       <c r="T36" s="62"/>
     </row>
-    <row r="37" spans="1:20" ht="12.9" customHeight="1">
+    <row r="37" spans="1:20" ht="12.95" customHeight="1">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -3355,7 +3411,7 @@
       <c r="S38" s="26"/>
       <c r="T38" s="62"/>
     </row>
-    <row r="39" spans="1:20" ht="15.9" customHeight="1">
+    <row r="39" spans="1:20" ht="15.95" customHeight="1">
       <c r="A39" s="13" t="s">
         <v>21</v>
       </c>
@@ -3382,7 +3438,7 @@
       <c r="S39" s="26"/>
       <c r="T39" s="62"/>
     </row>
-    <row r="40" spans="1:20" ht="15.9" customHeight="1">
+    <row r="40" spans="1:20" ht="15.95" customHeight="1">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -3404,7 +3460,7 @@
       <c r="S40" s="26"/>
       <c r="T40" s="62"/>
     </row>
-    <row r="41" spans="1:20" ht="15.9" customHeight="1">
+    <row r="41" spans="1:20" ht="15.95" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>24</v>
       </c>
@@ -3428,7 +3484,7 @@
       <c r="S41" s="26"/>
       <c r="T41" s="62"/>
     </row>
-    <row r="42" spans="1:20" ht="15.9" customHeight="1">
+    <row r="42" spans="1:20" ht="15.95" customHeight="1">
       <c r="A42" s="13" t="s">
         <v>25</v>
       </c>
@@ -3475,7 +3531,7 @@
     <row r="46" spans="1:20" ht="15" customHeight="1">
       <c r="M46" s="7"/>
     </row>
-    <row r="47" spans="1:20" ht="9.9" customHeight="1"/>
+    <row r="47" spans="1:20" ht="9.9499999999999993" customHeight="1"/>
     <row r="48" spans="1:20" ht="8.1" customHeight="1">
       <c r="N48" s="8" t="s">
         <v>26</v>
@@ -3552,7 +3608,7 @@
     </row>
     <row r="57" spans="1:20" ht="14.1" customHeight="1">
       <c r="A57" s="53" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B57" s="54"/>
       <c r="C57" s="54"/>
@@ -3562,7 +3618,7 @@
       <c r="G57" s="18"/>
       <c r="H57" s="18"/>
       <c r="I57" s="55" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="J57" s="54"/>
       <c r="K57" s="18"/>
@@ -3580,7 +3636,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="15.9" customHeight="1">
+    <row r="58" spans="1:20" ht="15.95" customHeight="1">
       <c r="A58" s="12"/>
       <c r="B58" s="12"/>
       <c r="C58" s="12"/>
@@ -3599,7 +3655,7 @@
       <c r="P58" s="12"/>
       <c r="Q58" s="12"/>
     </row>
-    <row r="59" spans="1:20" ht="15.9" customHeight="1">
+    <row r="59" spans="1:20" ht="15.95" customHeight="1">
       <c r="A59" s="84" t="s">
         <v>40</v>
       </c>
@@ -3623,7 +3679,7 @@
       <c r="S59" s="62"/>
       <c r="T59" s="62"/>
     </row>
-    <row r="60" spans="1:20" ht="15.9" customHeight="1">
+    <row r="60" spans="1:20" ht="15.95" customHeight="1">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -3642,7 +3698,7 @@
       <c r="P60" s="12"/>
       <c r="Q60" s="12"/>
     </row>
-    <row r="61" spans="1:20" ht="15.9" customHeight="1">
+    <row r="61" spans="1:20" ht="15.95" customHeight="1">
       <c r="A61" s="14" t="s">
         <v>41</v>
       </c>
@@ -3663,7 +3719,7 @@
       <c r="P61" s="12"/>
       <c r="Q61" s="12"/>
     </row>
-    <row r="62" spans="1:20" ht="15.9" customHeight="1">
+    <row r="62" spans="1:20" ht="15.95" customHeight="1">
       <c r="A62" s="28" t="s">
         <v>42</v>
       </c>
@@ -3686,7 +3742,7 @@
       <c r="P62" s="12"/>
       <c r="Q62" s="12"/>
     </row>
-    <row r="63" spans="1:20" ht="15.9" customHeight="1">
+    <row r="63" spans="1:20" ht="15.95" customHeight="1">
       <c r="A63" s="12"/>
       <c r="B63" s="12"/>
       <c r="C63" s="12"/>
@@ -3705,7 +3761,7 @@
       <c r="P63" s="12"/>
       <c r="Q63" s="12"/>
     </row>
-    <row r="64" spans="1:20" ht="15.9" customHeight="1">
+    <row r="64" spans="1:20" ht="15.95" customHeight="1">
       <c r="A64" s="15" t="s">
         <v>44</v>
       </c>
@@ -3752,7 +3808,7 @@
       <c r="S65" s="62"/>
       <c r="T65" s="62"/>
     </row>
-    <row r="66" spans="1:20" ht="15.9" customHeight="1">
+    <row r="66" spans="1:20" ht="15.95" customHeight="1">
       <c r="A66" s="12"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12"/>
@@ -3771,7 +3827,7 @@
       <c r="P66" s="12"/>
       <c r="Q66" s="12"/>
     </row>
-    <row r="67" spans="1:20" ht="15.9" customHeight="1">
+    <row r="67" spans="1:20" ht="15.95" customHeight="1">
       <c r="A67" s="23" t="s">
         <v>46</v>
       </c>
@@ -3844,12 +3900,12 @@
       <c r="S69" s="62"/>
       <c r="T69" s="62"/>
     </row>
-    <row r="71" spans="1:20" ht="15.9" customHeight="1">
+    <row r="71" spans="1:20" ht="15.95" customHeight="1">
       <c r="A71" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="15.9" customHeight="1">
+    <row r="72" spans="1:20" ht="15.95" customHeight="1">
       <c r="A72" s="28" t="s">
         <v>42</v>
       </c>
@@ -3872,15 +3928,15 @@
       <c r="P72" s="62"/>
       <c r="Q72" s="62"/>
     </row>
-    <row r="73" spans="1:20" ht="15.9" customHeight="1">
+    <row r="73" spans="1:20" ht="15.95" customHeight="1">
       <c r="A73" s="15"/>
     </row>
-    <row r="74" spans="1:20" ht="15.9" customHeight="1">
+    <row r="74" spans="1:20" ht="15.95" customHeight="1">
       <c r="A74" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="15.9" customHeight="1">
+    <row r="75" spans="1:20" ht="15.95" customHeight="1">
       <c r="A75" s="28" t="s">
         <v>42</v>
       </c>
@@ -3903,7 +3959,7 @@
       <c r="P75" s="62"/>
       <c r="Q75" s="62"/>
     </row>
-    <row r="76" spans="1:20" ht="15.9" customHeight="1">
+    <row r="76" spans="1:20" ht="15.95" customHeight="1">
       <c r="A76" s="28"/>
       <c r="B76" s="40"/>
       <c r="C76" s="40"/>
@@ -3922,7 +3978,7 @@
       <c r="P76" s="40"/>
       <c r="Q76" s="40"/>
     </row>
-    <row r="77" spans="1:20" ht="15.9" customHeight="1">
+    <row r="77" spans="1:20" ht="15.95" customHeight="1">
       <c r="A77" s="15"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
@@ -4007,7 +4063,7 @@
       <c r="P80" s="15"/>
       <c r="Q80" s="15"/>
     </row>
-    <row r="81" spans="1:20" ht="15.9" customHeight="1">
+    <row r="81" spans="1:20" ht="15.95" customHeight="1">
       <c r="A81" s="15" t="s">
         <v>54</v>
       </c>
@@ -4028,7 +4084,7 @@
       <c r="P81" s="15"/>
       <c r="Q81" s="15"/>
     </row>
-    <row r="82" spans="1:20" ht="63.9" customHeight="1" thickBot="1">
+    <row r="82" spans="1:20" ht="63.95" customHeight="1" thickBot="1">
       <c r="A82" s="16" t="s">
         <v>55</v>
       </c>
@@ -4073,8 +4129,8 @@
       <c r="P83" s="15"/>
       <c r="Q83" s="15"/>
     </row>
-    <row r="84" spans="1:20" ht="0.9" customHeight="1"/>
-    <row r="86" spans="1:20" ht="0.9" customHeight="1"/>
+    <row r="84" spans="1:20" ht="0.95" customHeight="1"/>
+    <row r="86" spans="1:20" ht="0.95" customHeight="1"/>
     <row r="87" spans="1:20" ht="17.100000000000001" customHeight="1"/>
     <row r="88" spans="1:20" ht="17.100000000000001" customHeight="1"/>
     <row r="89" spans="1:20" ht="17.100000000000001" customHeight="1"/>
@@ -4195,7 +4251,7 @@
       <c r="D110" s="26"/>
       <c r="E110" s="26"/>
       <c r="G110" s="50" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="H110" s="48"/>
       <c r="I110" s="48"/>
@@ -4217,7 +4273,7 @@
       <c r="D111" s="26"/>
       <c r="E111" s="26"/>
       <c r="G111" s="57" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="H111" s="48"/>
       <c r="I111" s="48"/>
@@ -4261,7 +4317,7 @@
       <c r="D113" s="26"/>
       <c r="E113" s="26"/>
       <c r="G113" s="58" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H113" s="48"/>
       <c r="I113" s="48"/>
@@ -4470,7 +4526,7 @@
       <c r="D123" s="26"/>
       <c r="E123" s="26"/>
       <c r="G123" s="48" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="H123" s="48"/>
       <c r="I123" s="48"/>
@@ -4504,7 +4560,7 @@
       <c r="P124" s="25"/>
       <c r="Q124" s="25"/>
     </row>
-    <row r="125" spans="1:20" s="28" customFormat="1" ht="9.9" customHeight="1">
+    <row r="125" spans="1:20" s="28" customFormat="1" ht="9.9499999999999993" customHeight="1">
       <c r="A125" s="25"/>
       <c r="B125" s="25"/>
       <c r="C125" s="25"/>
@@ -4523,7 +4579,7 @@
       <c r="P125" s="25"/>
       <c r="Q125" s="25"/>
     </row>
-    <row r="126" spans="1:20" ht="15.9" customHeight="1">
+    <row r="126" spans="1:20" ht="15.95" customHeight="1">
       <c r="A126" s="26"/>
       <c r="B126" s="26"/>
       <c r="C126" s="26"/>
@@ -4628,7 +4684,7 @@
     </row>
     <row r="129" spans="1:20" ht="20.25" customHeight="1">
       <c r="A129" s="161" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B129" s="91"/>
       <c r="C129" s="161">
@@ -4658,7 +4714,7 @@
       </c>
       <c r="P129" s="91"/>
       <c r="Q129" s="168">
-        <v>46.63</v>
+        <v>46.6</v>
       </c>
       <c r="R129" s="107"/>
       <c r="S129" s="155">
@@ -4668,7 +4724,7 @@
     </row>
     <row r="130" spans="1:20" ht="20.25" customHeight="1">
       <c r="A130" s="145" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B130" s="93"/>
       <c r="C130" s="145">
@@ -4698,7 +4754,7 @@
       </c>
       <c r="P130" s="93"/>
       <c r="Q130" s="149">
-        <v>46.69</v>
+        <v>46.74</v>
       </c>
       <c r="R130" s="100"/>
       <c r="S130" s="146">
@@ -4708,7 +4764,7 @@
     </row>
     <row r="131" spans="1:20" ht="20.25" customHeight="1">
       <c r="A131" s="150" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B131" s="93"/>
       <c r="C131" s="150">
@@ -4738,7 +4794,7 @@
       </c>
       <c r="P131" s="93"/>
       <c r="Q131" s="149">
-        <v>46.89</v>
+        <v>46.94</v>
       </c>
       <c r="R131" s="100"/>
       <c r="S131" s="143">
@@ -4748,7 +4804,7 @@
     </row>
     <row r="132" spans="1:20" ht="20.25" customHeight="1">
       <c r="A132" s="145" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B132" s="93"/>
       <c r="C132" s="145">
@@ -4778,7 +4834,7 @@
       </c>
       <c r="P132" s="93"/>
       <c r="Q132" s="149">
-        <v>47.03</v>
+        <v>47.12</v>
       </c>
       <c r="R132" s="100"/>
       <c r="S132" s="146">
@@ -4788,7 +4844,7 @@
     </row>
     <row r="133" spans="1:20" ht="20.25" customHeight="1">
       <c r="A133" s="150" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B133" s="93"/>
       <c r="C133" s="150">
@@ -4818,7 +4874,7 @@
       </c>
       <c r="P133" s="93"/>
       <c r="Q133" s="149">
-        <v>47.24</v>
+        <v>47.32</v>
       </c>
       <c r="R133" s="100"/>
       <c r="S133" s="143">
@@ -4828,7 +4884,7 @@
     </row>
     <row r="134" spans="1:20" ht="20.25" customHeight="1">
       <c r="A134" s="145" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B134" s="93"/>
       <c r="C134" s="145">
@@ -4858,7 +4914,7 @@
       </c>
       <c r="P134" s="93"/>
       <c r="Q134" s="149">
-        <v>47.53</v>
+        <v>47.63</v>
       </c>
       <c r="R134" s="100"/>
       <c r="S134" s="146">
@@ -4868,7 +4924,7 @@
     </row>
     <row r="135" spans="1:20" ht="20.25" customHeight="1">
       <c r="A135" s="150" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B135" s="93"/>
       <c r="C135" s="150">
@@ -4898,7 +4954,7 @@
       </c>
       <c r="P135" s="93"/>
       <c r="Q135" s="149">
-        <v>47.67</v>
+        <v>47.78</v>
       </c>
       <c r="R135" s="100"/>
       <c r="S135" s="143">
@@ -4908,7 +4964,7 @@
     </row>
     <row r="136" spans="1:20" ht="20.25" customHeight="1">
       <c r="A136" s="145" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B136" s="93"/>
       <c r="C136" s="145">
@@ -4938,7 +4994,7 @@
       </c>
       <c r="P136" s="93"/>
       <c r="Q136" s="149">
-        <v>47.72</v>
+        <v>47.82</v>
       </c>
       <c r="R136" s="100"/>
       <c r="S136" s="146">
@@ -4948,7 +5004,7 @@
     </row>
     <row r="137" spans="1:20" ht="20.25" customHeight="1">
       <c r="A137" s="150" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B137" s="93"/>
       <c r="C137" s="150">
@@ -4978,7 +5034,7 @@
       </c>
       <c r="P137" s="93"/>
       <c r="Q137" s="149">
-        <v>47.76</v>
+        <v>47.84</v>
       </c>
       <c r="R137" s="100"/>
       <c r="S137" s="143">
@@ -4988,7 +5044,7 @@
     </row>
     <row r="138" spans="1:20" ht="20.25" customHeight="1">
       <c r="A138" s="144" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B138" s="115"/>
       <c r="C138" s="145">
@@ -5018,7 +5074,7 @@
       </c>
       <c r="P138" s="93"/>
       <c r="Q138" s="149">
-        <v>47.66</v>
+        <v>47.76</v>
       </c>
       <c r="R138" s="100"/>
       <c r="S138" s="146">
@@ -5028,7 +5084,7 @@
     </row>
     <row r="139" spans="1:20" ht="14.1" customHeight="1">
       <c r="A139" s="139" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B139" s="66"/>
       <c r="C139" s="139">
@@ -5058,7 +5114,7 @@
       </c>
       <c r="P139" s="66"/>
       <c r="Q139" s="142">
-        <v>47.79</v>
+        <v>47.85</v>
       </c>
       <c r="R139" s="64"/>
       <c r="S139" s="136">
@@ -5153,7 +5209,7 @@
       <c r="S143" s="17"/>
     </row>
     <row r="144" spans="1:20" ht="15" customHeight="1" thickBot="1"/>
-    <row r="145" spans="1:21" ht="14.4" customHeight="1">
+    <row r="145" spans="1:21" ht="14.45" customHeight="1">
       <c r="A145" s="42" t="str">
         <f>A57</f>
         <v>Calibration No: CAL00001</v>
@@ -5314,7 +5370,7 @@
     </row>
     <row r="151" spans="1:21" ht="14.25" customHeight="1">
       <c r="A151" s="116" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B151" s="91"/>
       <c r="C151" s="116">
@@ -5342,7 +5398,7 @@
       </c>
       <c r="P151" s="91"/>
       <c r="Q151" s="106">
-        <v>51.05</v>
+        <v>51.03</v>
       </c>
       <c r="R151" s="107"/>
       <c r="S151" s="117">
@@ -5352,7 +5408,7 @@
     </row>
     <row r="152" spans="1:21" ht="14.25" customHeight="1">
       <c r="A152" s="109" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B152" s="93"/>
       <c r="C152" s="109">
@@ -5380,7 +5436,7 @@
       </c>
       <c r="P152" s="93"/>
       <c r="Q152" s="99">
-        <v>48.8</v>
+        <v>48.78</v>
       </c>
       <c r="R152" s="100"/>
       <c r="S152" s="108">
@@ -5390,7 +5446,7 @@
     </row>
     <row r="153" spans="1:21" ht="14.25" customHeight="1">
       <c r="A153" s="129" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B153" s="115"/>
       <c r="C153" s="129">
@@ -5420,7 +5476,7 @@
       </c>
       <c r="P153" s="115"/>
       <c r="Q153" s="127">
-        <v>46.76</v>
+        <v>46.72</v>
       </c>
       <c r="R153" s="128"/>
       <c r="S153" s="130">
@@ -5430,7 +5486,7 @@
     </row>
     <row r="154" spans="1:21" ht="14.25" customHeight="1">
       <c r="A154" s="101" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B154" s="91"/>
       <c r="C154" s="101">
@@ -5458,7 +5514,7 @@
       </c>
       <c r="P154" s="91"/>
       <c r="Q154" s="106">
-        <v>50.27</v>
+        <v>50.26</v>
       </c>
       <c r="R154" s="107"/>
       <c r="S154" s="90">
@@ -5468,7 +5524,7 @@
     </row>
     <row r="155" spans="1:21" ht="14.25" customHeight="1">
       <c r="A155" s="92" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B155" s="93"/>
       <c r="C155" s="92">
@@ -5496,7 +5552,7 @@
       </c>
       <c r="P155" s="93"/>
       <c r="Q155" s="99">
-        <v>48.31</v>
+        <v>48.32</v>
       </c>
       <c r="R155" s="100"/>
       <c r="S155" s="94">
@@ -5506,7 +5562,7 @@
     </row>
     <row r="156" spans="1:21" ht="14.25" customHeight="1">
       <c r="A156" s="109" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="B156" s="93"/>
       <c r="C156" s="109">
@@ -5536,7 +5592,7 @@
       </c>
       <c r="P156" s="93"/>
       <c r="Q156" s="99">
-        <v>46.63</v>
+        <v>46.6</v>
       </c>
       <c r="R156" s="100"/>
       <c r="S156" s="108">
@@ -5546,7 +5602,7 @@
     </row>
     <row r="157" spans="1:21" ht="14.25" customHeight="1">
       <c r="A157" s="129" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B157" s="115"/>
       <c r="C157" s="129">
@@ -5576,7 +5632,7 @@
       </c>
       <c r="P157" s="115"/>
       <c r="Q157" s="127">
-        <v>46.5</v>
+        <v>46.51</v>
       </c>
       <c r="R157" s="128"/>
       <c r="S157" s="130">
@@ -5586,7 +5642,7 @@
     </row>
     <row r="158" spans="1:21" ht="14.25" customHeight="1">
       <c r="A158" s="101" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B158" s="91"/>
       <c r="C158" s="101">
@@ -5624,7 +5680,7 @@
     </row>
     <row r="159" spans="1:21" ht="14.25" customHeight="1">
       <c r="A159" s="92" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B159" s="93"/>
       <c r="C159" s="92">
@@ -5652,7 +5708,7 @@
       </c>
       <c r="P159" s="93"/>
       <c r="Q159" s="99">
-        <v>48.04</v>
+        <v>48.06</v>
       </c>
       <c r="R159" s="100"/>
       <c r="S159" s="94">
@@ -5662,7 +5718,7 @@
     </row>
     <row r="160" spans="1:21" ht="14.25" customHeight="1">
       <c r="A160" s="122" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B160" s="115"/>
       <c r="C160" s="122">
@@ -5692,7 +5748,7 @@
       </c>
       <c r="P160" s="115"/>
       <c r="Q160" s="127">
-        <v>46.67</v>
+        <v>46.7</v>
       </c>
       <c r="R160" s="128"/>
       <c r="S160" s="114">
@@ -5702,7 +5758,7 @@
     </row>
     <row r="161" spans="1:20" ht="14.25" customHeight="1">
       <c r="A161" s="116" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B161" s="91"/>
       <c r="C161" s="116">
@@ -5730,7 +5786,7 @@
       </c>
       <c r="P161" s="91"/>
       <c r="Q161" s="106">
-        <v>49.37</v>
+        <v>49.35</v>
       </c>
       <c r="R161" s="107"/>
       <c r="S161" s="117">
@@ -5740,7 +5796,7 @@
     </row>
     <row r="162" spans="1:20" ht="14.25" customHeight="1">
       <c r="A162" s="109" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B162" s="93"/>
       <c r="C162" s="109">
@@ -5768,7 +5824,7 @@
       </c>
       <c r="P162" s="93"/>
       <c r="Q162" s="99">
-        <v>47.84</v>
+        <v>47.87</v>
       </c>
       <c r="R162" s="100"/>
       <c r="S162" s="108">
@@ -5778,7 +5834,7 @@
     </row>
     <row r="163" spans="1:20" ht="14.25" customHeight="1">
       <c r="A163" s="92" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B163" s="93"/>
       <c r="C163" s="92">
@@ -5808,7 +5864,7 @@
       </c>
       <c r="P163" s="93"/>
       <c r="Q163" s="99">
-        <v>46.69</v>
+        <v>46.74</v>
       </c>
       <c r="R163" s="100"/>
       <c r="S163" s="94">
@@ -5818,7 +5874,7 @@
     </row>
     <row r="164" spans="1:20" ht="14.25" customHeight="1">
       <c r="A164" s="109" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B164" s="93"/>
       <c r="C164" s="109">
@@ -5848,7 +5904,7 @@
       </c>
       <c r="P164" s="93"/>
       <c r="Q164" s="99">
-        <v>46.65</v>
+        <v>46.7</v>
       </c>
       <c r="R164" s="100"/>
       <c r="S164" s="108">
@@ -5858,7 +5914,7 @@
     </row>
     <row r="165" spans="1:20" ht="14.25" customHeight="1">
       <c r="A165" s="92" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="B165" s="93"/>
       <c r="C165" s="92">
@@ -5888,7 +5944,7 @@
       </c>
       <c r="P165" s="93"/>
       <c r="Q165" s="99">
-        <v>46.59</v>
+        <v>46.63</v>
       </c>
       <c r="R165" s="100"/>
       <c r="S165" s="94">
@@ -5898,7 +5954,7 @@
     </row>
     <row r="166" spans="1:20" ht="14.25" customHeight="1">
       <c r="A166" s="101" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B166" s="91"/>
       <c r="C166" s="101">
@@ -5926,7 +5982,7 @@
       </c>
       <c r="P166" s="91"/>
       <c r="Q166" s="106">
-        <v>49.05</v>
+        <v>49.06</v>
       </c>
       <c r="R166" s="107"/>
       <c r="S166" s="90">
@@ -5936,7 +5992,7 @@
     </row>
     <row r="167" spans="1:20" ht="14.25" customHeight="1">
       <c r="A167" s="92" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B167" s="93"/>
       <c r="C167" s="92">
@@ -5964,7 +6020,7 @@
       </c>
       <c r="P167" s="93"/>
       <c r="Q167" s="99">
-        <v>47.73</v>
+        <v>47.74</v>
       </c>
       <c r="R167" s="100"/>
       <c r="S167" s="94">
@@ -5974,7 +6030,7 @@
     </row>
     <row r="168" spans="1:20" ht="14.25" customHeight="1">
       <c r="A168" s="122" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B168" s="115"/>
       <c r="C168" s="122">
@@ -6004,7 +6060,7 @@
       </c>
       <c r="P168" s="115"/>
       <c r="Q168" s="127">
-        <v>46.74</v>
+        <v>46.8</v>
       </c>
       <c r="R168" s="128"/>
       <c r="S168" s="114">
@@ -6014,7 +6070,7 @@
     </row>
     <row r="169" spans="1:20" ht="14.25" customHeight="1">
       <c r="A169" s="116" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B169" s="91"/>
       <c r="C169" s="116">
@@ -6042,7 +6098,7 @@
       </c>
       <c r="P169" s="91"/>
       <c r="Q169" s="106">
-        <v>48.78</v>
+        <v>48.8</v>
       </c>
       <c r="R169" s="107"/>
       <c r="S169" s="117">
@@ -6052,7 +6108,7 @@
     </row>
     <row r="170" spans="1:20" ht="14.25" customHeight="1">
       <c r="A170" s="109" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B170" s="93"/>
       <c r="C170" s="109">
@@ -6090,7 +6146,7 @@
     </row>
     <row r="171" spans="1:20" ht="14.25" customHeight="1">
       <c r="A171" s="92" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B171" s="93"/>
       <c r="C171" s="92">
@@ -6120,7 +6176,7 @@
       </c>
       <c r="P171" s="93"/>
       <c r="Q171" s="99">
-        <v>46.81</v>
+        <v>46.89</v>
       </c>
       <c r="R171" s="100"/>
       <c r="S171" s="94">
@@ -6130,7 +6186,7 @@
     </row>
     <row r="172" spans="1:20" ht="14.25" customHeight="1">
       <c r="A172" s="101" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B172" s="91"/>
       <c r="C172" s="101">
@@ -6158,7 +6214,7 @@
       </c>
       <c r="P172" s="91"/>
       <c r="Q172" s="106">
-        <v>48.63</v>
+        <v>48.59</v>
       </c>
       <c r="R172" s="107"/>
       <c r="S172" s="90">
@@ -6168,7 +6224,7 @@
     </row>
     <row r="173" spans="1:20" ht="14.25" customHeight="1">
       <c r="A173" s="92" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B173" s="93"/>
       <c r="C173" s="92">
@@ -6206,7 +6262,7 @@
     </row>
     <row r="174" spans="1:20" ht="14.25" customHeight="1">
       <c r="A174" s="109" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B174" s="93"/>
       <c r="C174" s="109">
@@ -6236,7 +6292,7 @@
       </c>
       <c r="P174" s="93"/>
       <c r="Q174" s="99">
-        <v>46.89</v>
+        <v>46.94</v>
       </c>
       <c r="R174" s="100"/>
       <c r="S174" s="108">
@@ -6246,7 +6302,7 @@
     </row>
     <row r="175" spans="1:20" ht="14.25" customHeight="1">
       <c r="A175" s="92" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="B175" s="93"/>
       <c r="C175" s="92">
@@ -6276,7 +6332,7 @@
       </c>
       <c r="P175" s="93"/>
       <c r="Q175" s="99">
-        <v>46.96</v>
+        <v>47.02</v>
       </c>
       <c r="R175" s="100"/>
       <c r="S175" s="94">
@@ -6286,7 +6342,7 @@
     </row>
     <row r="176" spans="1:20" ht="14.25" customHeight="1">
       <c r="A176" s="122" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="B176" s="115"/>
       <c r="C176" s="122">
@@ -6316,7 +6372,7 @@
       </c>
       <c r="P176" s="115"/>
       <c r="Q176" s="127">
-        <v>47.04</v>
+        <v>47.12</v>
       </c>
       <c r="R176" s="128"/>
       <c r="S176" s="114">
@@ -6326,7 +6382,7 @@
     </row>
     <row r="177" spans="1:20" ht="14.25" customHeight="1">
       <c r="A177" s="92" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B177" s="93"/>
       <c r="C177" s="92">
@@ -6356,7 +6412,7 @@
       </c>
       <c r="P177" s="93"/>
       <c r="Q177" s="99">
-        <v>46.98</v>
+        <v>47.04</v>
       </c>
       <c r="R177" s="100"/>
       <c r="S177" s="94">
@@ -6366,7 +6422,7 @@
     </row>
     <row r="178" spans="1:20" ht="14.25" customHeight="1">
       <c r="A178" s="109" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="B178" s="93"/>
       <c r="C178" s="109">
@@ -6396,7 +6452,7 @@
       </c>
       <c r="P178" s="93"/>
       <c r="Q178" s="99">
-        <v>47.03</v>
+        <v>47.12</v>
       </c>
       <c r="R178" s="100"/>
       <c r="S178" s="108">
@@ -6406,7 +6462,7 @@
     </row>
     <row r="179" spans="1:20" ht="14.25" customHeight="1">
       <c r="A179" s="92" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B179" s="93"/>
       <c r="C179" s="92">
@@ -6436,7 +6492,7 @@
       </c>
       <c r="P179" s="93"/>
       <c r="Q179" s="99">
-        <v>47.19</v>
+        <v>47.24</v>
       </c>
       <c r="R179" s="100"/>
       <c r="S179" s="94">
@@ -6446,7 +6502,7 @@
     </row>
     <row r="180" spans="1:20" ht="14.25" customHeight="1">
       <c r="A180" s="122" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B180" s="115"/>
       <c r="C180" s="122">
@@ -6478,7 +6534,7 @@
       </c>
       <c r="P180" s="115"/>
       <c r="Q180" s="127">
-        <v>47.49</v>
+        <v>47.56</v>
       </c>
       <c r="R180" s="128"/>
       <c r="S180" s="114">
@@ -6488,7 +6544,7 @@
     </row>
     <row r="181" spans="1:20" ht="14.25" customHeight="1">
       <c r="A181" s="116" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B181" s="91"/>
       <c r="C181" s="116">
@@ -6518,7 +6574,7 @@
       </c>
       <c r="P181" s="91"/>
       <c r="Q181" s="106">
-        <v>47.02</v>
+        <v>47.1</v>
       </c>
       <c r="R181" s="107"/>
       <c r="S181" s="117">
@@ -6528,7 +6584,7 @@
     </row>
     <row r="182" spans="1:20" ht="14.25" customHeight="1">
       <c r="A182" s="109" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B182" s="93"/>
       <c r="C182" s="109">
@@ -6558,7 +6614,7 @@
       </c>
       <c r="P182" s="93"/>
       <c r="Q182" s="99">
-        <v>47.11</v>
+        <v>47.18</v>
       </c>
       <c r="R182" s="100"/>
       <c r="S182" s="108">
@@ -6568,7 +6624,7 @@
     </row>
     <row r="183" spans="1:20" ht="14.25" customHeight="1">
       <c r="A183" s="92" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="B183" s="93"/>
       <c r="C183" s="92">
@@ -6598,7 +6654,7 @@
       </c>
       <c r="P183" s="93"/>
       <c r="Q183" s="99">
-        <v>47.24</v>
+        <v>47.32</v>
       </c>
       <c r="R183" s="100"/>
       <c r="S183" s="94">
@@ -6608,7 +6664,7 @@
     </row>
     <row r="184" spans="1:20" ht="14.25" customHeight="1">
       <c r="A184" s="109" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B184" s="93"/>
       <c r="C184" s="109">
@@ -6638,7 +6694,7 @@
       </c>
       <c r="P184" s="93"/>
       <c r="Q184" s="99">
-        <v>47.52</v>
+        <v>47.62</v>
       </c>
       <c r="R184" s="100"/>
       <c r="S184" s="108">
@@ -6648,7 +6704,7 @@
     </row>
     <row r="185" spans="1:20" ht="14.25" customHeight="1">
       <c r="A185" s="129" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B185" s="115"/>
       <c r="C185" s="129">
@@ -6678,7 +6734,7 @@
       </c>
       <c r="P185" s="115"/>
       <c r="Q185" s="127">
-        <v>47.64</v>
+        <v>47.7</v>
       </c>
       <c r="R185" s="128"/>
       <c r="S185" s="130">
@@ -6688,7 +6744,7 @@
     </row>
     <row r="186" spans="1:20" ht="14.25" customHeight="1">
       <c r="A186" s="101" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B186" s="91"/>
       <c r="C186" s="101">
@@ -6718,7 +6774,7 @@
       </c>
       <c r="P186" s="91"/>
       <c r="Q186" s="106">
-        <v>47.14</v>
+        <v>47.21</v>
       </c>
       <c r="R186" s="107"/>
       <c r="S186" s="90">
@@ -6728,7 +6784,7 @@
     </row>
     <row r="187" spans="1:20" ht="14.25" customHeight="1">
       <c r="A187" s="92" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B187" s="93"/>
       <c r="C187" s="92">
@@ -6758,7 +6814,7 @@
       </c>
       <c r="P187" s="93"/>
       <c r="Q187" s="99">
-        <v>47.28</v>
+        <v>47.36</v>
       </c>
       <c r="R187" s="100"/>
       <c r="S187" s="94">
@@ -6768,7 +6824,7 @@
     </row>
     <row r="188" spans="1:20" ht="14.25" customHeight="1">
       <c r="A188" s="109" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B188" s="93"/>
       <c r="C188" s="109">
@@ -6798,7 +6854,7 @@
       </c>
       <c r="P188" s="93"/>
       <c r="Q188" s="99">
-        <v>47.53</v>
+        <v>47.63</v>
       </c>
       <c r="R188" s="100"/>
       <c r="S188" s="108">
@@ -6808,7 +6864,7 @@
     </row>
     <row r="189" spans="1:20" ht="14.1" customHeight="1">
       <c r="A189" s="92" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B189" s="93"/>
       <c r="C189" s="92">
@@ -6838,7 +6894,7 @@
       </c>
       <c r="P189" s="93"/>
       <c r="Q189" s="99">
-        <v>47.64</v>
+        <v>47.74</v>
       </c>
       <c r="R189" s="100"/>
       <c r="S189" s="94">
@@ -6848,7 +6904,7 @@
     </row>
     <row r="190" spans="1:20" ht="16.5" customHeight="1">
       <c r="A190" s="122" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B190" s="115"/>
       <c r="C190" s="122">
@@ -6878,7 +6934,7 @@
       </c>
       <c r="P190" s="115"/>
       <c r="Q190" s="127">
-        <v>47.63</v>
+        <v>47.72</v>
       </c>
       <c r="R190" s="128"/>
       <c r="S190" s="114">
@@ -6886,7 +6942,7 @@
       </c>
       <c r="T190" s="115"/>
     </row>
-    <row r="191" spans="1:20" ht="7.8" customHeight="1"/>
+    <row r="191" spans="1:20" ht="7.9" customHeight="1"/>
     <row r="192" spans="1:20" ht="21" customHeight="1">
       <c r="P192" s="22" t="s">
         <v>99</v>
@@ -7031,7 +7087,7 @@
     </row>
     <row r="198" spans="1:20" ht="14.25" customHeight="1">
       <c r="A198" s="116" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
       <c r="B198" s="91"/>
       <c r="C198" s="116">
@@ -7061,7 +7117,7 @@
       </c>
       <c r="P198" s="91"/>
       <c r="Q198" s="106">
-        <v>47.36</v>
+        <v>47.47</v>
       </c>
       <c r="R198" s="107"/>
       <c r="S198" s="117">
@@ -7071,7 +7127,7 @@
     </row>
     <row r="199" spans="1:20" ht="14.25" customHeight="1">
       <c r="A199" s="109" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="B199" s="93"/>
       <c r="C199" s="109">
@@ -7101,7 +7157,7 @@
       </c>
       <c r="P199" s="93"/>
       <c r="Q199" s="99">
-        <v>47.58</v>
+        <v>47.68</v>
       </c>
       <c r="R199" s="100"/>
       <c r="S199" s="108">
@@ -7111,7 +7167,7 @@
     </row>
     <row r="200" spans="1:20" ht="14.25" customHeight="1">
       <c r="A200" s="92" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B200" s="93"/>
       <c r="C200" s="92">
@@ -7141,7 +7197,7 @@
       </c>
       <c r="P200" s="93"/>
       <c r="Q200" s="99">
-        <v>47.67</v>
+        <v>47.78</v>
       </c>
       <c r="R200" s="100"/>
       <c r="S200" s="94">
@@ -7151,7 +7207,7 @@
     </row>
     <row r="201" spans="1:20" ht="14.25" customHeight="1">
       <c r="A201" s="109" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B201" s="93"/>
       <c r="C201" s="109">
@@ -7181,7 +7237,7 @@
       </c>
       <c r="P201" s="93"/>
       <c r="Q201" s="99">
-        <v>47.72</v>
+        <v>47.8</v>
       </c>
       <c r="R201" s="100"/>
       <c r="S201" s="108">
@@ -7191,7 +7247,7 @@
     </row>
     <row r="202" spans="1:20" ht="14.25" customHeight="1">
       <c r="A202" s="129" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B202" s="115"/>
       <c r="C202" s="129">
@@ -7221,7 +7277,7 @@
       </c>
       <c r="P202" s="115"/>
       <c r="Q202" s="127">
-        <v>47.69</v>
+        <v>47.78</v>
       </c>
       <c r="R202" s="128"/>
       <c r="S202" s="130">
@@ -7231,7 +7287,7 @@
     </row>
     <row r="203" spans="1:20" ht="14.25" customHeight="1">
       <c r="A203" s="101" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B203" s="91"/>
       <c r="C203" s="101">
@@ -7261,7 +7317,7 @@
       </c>
       <c r="P203" s="91"/>
       <c r="Q203" s="106">
-        <v>47.61</v>
+        <v>47.72</v>
       </c>
       <c r="R203" s="107"/>
       <c r="S203" s="90">
@@ -7271,7 +7327,7 @@
     </row>
     <row r="204" spans="1:20" ht="14.25" customHeight="1">
       <c r="A204" s="92" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B204" s="93"/>
       <c r="C204" s="92">
@@ -7301,7 +7357,7 @@
       </c>
       <c r="P204" s="93"/>
       <c r="Q204" s="99">
-        <v>47.69</v>
+        <v>47.78</v>
       </c>
       <c r="R204" s="100"/>
       <c r="S204" s="94">
@@ -7311,7 +7367,7 @@
     </row>
     <row r="205" spans="1:20" ht="14.25" customHeight="1">
       <c r="A205" s="109" t="s">
-        <v>123</v>
+        <v>173</v>
       </c>
       <c r="B205" s="93"/>
       <c r="C205" s="109">
@@ -7341,7 +7397,7 @@
       </c>
       <c r="P205" s="93"/>
       <c r="Q205" s="99">
-        <v>47.72</v>
+        <v>47.82</v>
       </c>
       <c r="R205" s="100"/>
       <c r="S205" s="108">
@@ -7351,7 +7407,7 @@
     </row>
     <row r="206" spans="1:20" ht="14.25" customHeight="1">
       <c r="A206" s="92" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B206" s="93"/>
       <c r="C206" s="92">
@@ -7381,7 +7437,7 @@
       </c>
       <c r="P206" s="93"/>
       <c r="Q206" s="99">
-        <v>47.79</v>
+        <v>47.88</v>
       </c>
       <c r="R206" s="100"/>
       <c r="S206" s="94">
@@ -7391,7 +7447,7 @@
     </row>
     <row r="207" spans="1:20" ht="14.25" customHeight="1">
       <c r="A207" s="122" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B207" s="115"/>
       <c r="C207" s="122">
@@ -7421,7 +7477,7 @@
       </c>
       <c r="P207" s="115"/>
       <c r="Q207" s="127">
-        <v>47.75</v>
+        <v>47.85</v>
       </c>
       <c r="R207" s="128"/>
       <c r="S207" s="114">
@@ -7431,7 +7487,7 @@
     </row>
     <row r="208" spans="1:20" ht="14.25" customHeight="1">
       <c r="A208" s="92" t="s">
-        <v>169</v>
+        <v>114</v>
       </c>
       <c r="B208" s="93"/>
       <c r="C208" s="92">
@@ -7461,7 +7517,7 @@
       </c>
       <c r="P208" s="93"/>
       <c r="Q208" s="99">
-        <v>47.69</v>
+        <v>47.78</v>
       </c>
       <c r="R208" s="100"/>
       <c r="S208" s="94">
@@ -7471,7 +7527,7 @@
     </row>
     <row r="209" spans="1:20" ht="14.25" customHeight="1">
       <c r="A209" s="109" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B209" s="93"/>
       <c r="C209" s="109">
@@ -7501,7 +7557,7 @@
       </c>
       <c r="P209" s="93"/>
       <c r="Q209" s="99">
-        <v>47.69</v>
+        <v>47.8</v>
       </c>
       <c r="R209" s="100"/>
       <c r="S209" s="108">
@@ -7511,7 +7567,7 @@
     </row>
     <row r="210" spans="1:20" ht="14.25" customHeight="1">
       <c r="A210" s="92" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B210" s="93"/>
       <c r="C210" s="92">
@@ -7541,7 +7597,7 @@
       </c>
       <c r="P210" s="93"/>
       <c r="Q210" s="99">
-        <v>47.76</v>
+        <v>47.84</v>
       </c>
       <c r="R210" s="100"/>
       <c r="S210" s="94">
@@ -7551,7 +7607,7 @@
     </row>
     <row r="211" spans="1:20" ht="14.25" customHeight="1">
       <c r="A211" s="122" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B211" s="115"/>
       <c r="C211" s="122">
@@ -7581,7 +7637,7 @@
       </c>
       <c r="P211" s="115"/>
       <c r="Q211" s="127">
-        <v>47.76</v>
+        <v>47.82</v>
       </c>
       <c r="R211" s="128"/>
       <c r="S211" s="114">
@@ -7591,7 +7647,7 @@
     </row>
     <row r="212" spans="1:20" ht="14.25" customHeight="1">
       <c r="A212" s="116" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="B212" s="91"/>
       <c r="C212" s="116">
@@ -7621,7 +7677,7 @@
       </c>
       <c r="P212" s="91"/>
       <c r="Q212" s="106">
-        <v>47.64</v>
+        <v>47.74</v>
       </c>
       <c r="R212" s="107"/>
       <c r="S212" s="117">
@@ -7631,7 +7687,7 @@
     </row>
     <row r="213" spans="1:20" ht="14.25" customHeight="1">
       <c r="A213" s="109" t="s">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="B213" s="93"/>
       <c r="C213" s="109">
@@ -7661,7 +7717,7 @@
       </c>
       <c r="P213" s="93"/>
       <c r="Q213" s="99">
-        <v>47.66</v>
+        <v>47.76</v>
       </c>
       <c r="R213" s="100"/>
       <c r="S213" s="108">
@@ -7671,7 +7727,7 @@
     </row>
     <row r="214" spans="1:20" ht="14.25" customHeight="1">
       <c r="A214" s="92" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B214" s="93"/>
       <c r="C214" s="92">
@@ -7701,7 +7757,7 @@
       </c>
       <c r="P214" s="93"/>
       <c r="Q214" s="99">
-        <v>47.69</v>
+        <v>47.74</v>
       </c>
       <c r="R214" s="100"/>
       <c r="S214" s="94">
@@ -7711,7 +7767,7 @@
     </row>
     <row r="215" spans="1:20" ht="14.25" customHeight="1">
       <c r="A215" s="101" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B215" s="91"/>
       <c r="C215" s="101">
@@ -7741,7 +7797,7 @@
       </c>
       <c r="P215" s="91"/>
       <c r="Q215" s="106">
-        <v>47.57</v>
+        <v>47.66</v>
       </c>
       <c r="R215" s="107"/>
       <c r="S215" s="90">
@@ -7751,7 +7807,7 @@
     </row>
     <row r="216" spans="1:20" ht="14.25" customHeight="1">
       <c r="A216" s="92" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B216" s="93"/>
       <c r="C216" s="92">
@@ -7781,7 +7837,7 @@
       </c>
       <c r="P216" s="93"/>
       <c r="Q216" s="99">
-        <v>47.58</v>
+        <v>47.66</v>
       </c>
       <c r="R216" s="100"/>
       <c r="S216" s="94">
@@ -7791,7 +7847,7 @@
     </row>
     <row r="217" spans="1:20" ht="15" customHeight="1">
       <c r="A217" s="69" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B217" s="66"/>
       <c r="C217" s="69">
@@ -7821,7 +7877,7 @@
       </c>
       <c r="P217" s="66"/>
       <c r="Q217" s="63">
-        <v>47.64</v>
+        <v>47.69</v>
       </c>
       <c r="R217" s="64"/>
       <c r="S217" s="65">
@@ -7831,7 +7887,7 @@
     </row>
     <row r="218" spans="1:20" ht="15" customHeight="1">
       <c r="A218" s="74" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B218" s="66"/>
       <c r="C218" s="74">
@@ -7861,7 +7917,7 @@
       </c>
       <c r="P218" s="66"/>
       <c r="Q218" s="63">
-        <v>47.82</v>
+        <v>47.87</v>
       </c>
       <c r="R218" s="64"/>
       <c r="S218" s="68">
@@ -7871,7 +7927,7 @@
     </row>
     <row r="219" spans="1:20" ht="15" customHeight="1">
       <c r="A219" s="69" t="s">
-        <v>126</v>
+        <v>185</v>
       </c>
       <c r="B219" s="66"/>
       <c r="C219" s="69">
@@ -7901,7 +7957,7 @@
       </c>
       <c r="P219" s="66"/>
       <c r="Q219" s="63">
-        <v>47.79</v>
+        <v>47.85</v>
       </c>
       <c r="R219" s="64"/>
       <c r="S219" s="65">
@@ -7969,7 +8025,7 @@
       <c r="S243" s="62"/>
       <c r="T243" s="62"/>
     </row>
-    <row r="245" spans="1:20" s="60" customFormat="1" ht="13.8" thickBot="1"/>
+    <row r="245" spans="1:20" s="60" customFormat="1" ht="13.5" thickBot="1"/>
     <row r="246" spans="1:20" s="60" customFormat="1">
       <c r="A246" s="42" t="str">
         <f>A57</f>
@@ -8056,7 +8112,7 @@
     <row r="303" spans="1:20" ht="14.1" customHeight="1"/>
     <row r="304" spans="1:20" s="47" customFormat="1"/>
     <row r="306" spans="1:20" ht="15" customHeight="1"/>
-    <row r="307" spans="1:20" ht="13.8" thickBot="1"/>
+    <row r="307" spans="1:20" ht="13.5" thickBot="1"/>
     <row r="308" spans="1:20">
       <c r="A308" s="42" t="str">
         <f>A57</f>

</xml_diff>